<commit_message>
creando formularios de prueba
</commit_message>
<xml_diff>
--- a/campeonato.xlsx
+++ b/campeonato.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Campeonato\proyectoCampeonato\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A320868-3010-4268-8241-391D1F644E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1BF1D66-B75A-47A2-819F-48CBCAC12517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="8" r:id="rId1"/>
@@ -30,7 +30,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId8"/>
+    <pivotCache cacheId="4" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -706,7 +706,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Asus" refreshedDate="45954.555560995374" refreshedVersion="8" recordCount="16" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Asus" refreshedDate="45954.597264467593" refreshedVersion="8" recordCount="16" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:F1000" sheet="4. Resultados acumulados"/>
   </cacheSource>
@@ -886,7 +886,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0600-000000000000}" name="5. Tabla de posiciones" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="8" compact="0" compactData="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0600-000000000000}" name="5. Tabla de posiciones" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="8" compact="0" compactData="0">
   <location ref="A1:F16" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField name="Equipo" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="descending">
@@ -1203,9 +1203,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{016E49F4-1090-408C-AE80-D664AD544DA1}">
+  <sheetPr codeName="Hoja1"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1217,12 +1218,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Hoja2">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -1427,7 +1428,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Hoja3">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:E56"/>
@@ -2400,7 +2401,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Hoja4">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:L21"/>
@@ -2874,7 +2875,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Hoja5">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:J19"/>
@@ -3249,7 +3250,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Hoja6">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:F16"/>
@@ -3260,7 +3261,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="13.2">
       <c r="A1" s="18"/>
       <c r="B1" s="19" t="s">
         <v>118</v>
@@ -3270,7 +3271,7 @@
       <c r="E1" s="20"/>
       <c r="F1" s="21"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="13.2">
       <c r="A2" s="19" t="s">
         <v>25</v>
       </c>
@@ -3290,7 +3291,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" ht="13.2">
       <c r="A3" s="18" t="s">
         <v>21</v>
       </c>
@@ -3310,7 +3311,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" ht="13.2">
       <c r="A4" s="27" t="s">
         <v>12</v>
       </c>
@@ -3330,7 +3331,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" ht="13.2">
       <c r="A5" s="27" t="s">
         <v>7</v>
       </c>
@@ -3350,7 +3351,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="13.2">
       <c r="A6" s="27" t="s">
         <v>17</v>
       </c>
@@ -3370,7 +3371,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" ht="13.2">
       <c r="A7" s="27" t="s">
         <v>22</v>
       </c>
@@ -3390,7 +3391,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" ht="13.2">
       <c r="A8" s="27" t="s">
         <v>9</v>
       </c>
@@ -3410,7 +3411,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" ht="13.2">
       <c r="A9" s="27" t="s">
         <v>16</v>
       </c>
@@ -3430,7 +3431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="13.2">
       <c r="A10" s="27" t="s">
         <v>19</v>
       </c>
@@ -3450,7 +3451,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" ht="13.2">
       <c r="A11" s="27" t="s">
         <v>18</v>
       </c>
@@ -3470,7 +3471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" ht="13.2">
       <c r="A12" s="27" t="s">
         <v>14</v>
       </c>
@@ -3490,7 +3491,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" ht="13.2">
       <c r="A13" s="27" t="s">
         <v>20</v>
       </c>
@@ -3510,7 +3511,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" ht="13.2">
       <c r="A14" s="27" t="s">
         <v>4</v>
       </c>
@@ -3530,7 +3531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" ht="13.2">
       <c r="A15" s="27" t="s">
         <v>124</v>
       </c>
@@ -3567,7 +3568,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Hoja7">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:E8"/>

</xml_diff>

<commit_message>
agregado el formulario para agregar equipos
</commit_message>
<xml_diff>
--- a/campeonato.xlsx
+++ b/campeonato.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Campeonato\proyectoCampeonato\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Pedro0\proyectoCampeonato\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1BF1D66-B75A-47A2-819F-48CBCAC12517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323741B0-8211-4756-BCA1-C365CE0B2EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="8" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="6. Sanciones y tarjetas" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'1. Equipos'!$A$1:$D$1000</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'1. Equipos'!$A$1:$D$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2. Jugadores'!$A$1:$E$1000</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'3. Fixture'!$A$1:$G$1000</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'4. Resultados acumulados'!$A$1:$F$1000</definedName>
@@ -32,24 +32,11 @@
   <pivotCaches>
     <pivotCache cacheId="4" r:id="rId8"/>
   </pivotCaches>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="128">
   <si>
     <t>Nombre de promoción</t>
   </si>
@@ -427,6 +414,12 @@
   </si>
   <si>
     <t>Total general</t>
+  </si>
+  <si>
+    <t>asdasD</t>
+  </si>
+  <si>
+    <t>dfgsdgfsdfg</t>
   </si>
 </sst>
 </file>
@@ -514,11 +507,11 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFABABAB"/>
+        <color rgb="FF999999"/>
       </left>
       <right/>
       <top style="thin">
-        <color rgb="FFABABAB"/>
+        <color rgb="FF999999"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -529,7 +522,7 @@
       </left>
       <right/>
       <top style="thin">
-        <color rgb="FFABABAB"/>
+        <color rgb="FF999999"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -539,10 +532,10 @@
         <color indexed="65"/>
       </left>
       <right style="thin">
-        <color rgb="FFABABAB"/>
+        <color rgb="FF999999"/>
       </right>
       <top style="thin">
-        <color rgb="FFABABAB"/>
+        <color rgb="FF999999"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -551,7 +544,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color rgb="FFABABAB"/>
+        <color rgb="FF999999"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -559,17 +552,17 @@
     <border>
       <left/>
       <right style="thin">
-        <color rgb="FFABABAB"/>
+        <color rgb="FF999999"/>
       </right>
       <top style="thin">
-        <color rgb="FFABABAB"/>
+        <color rgb="FF999999"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFABABAB"/>
+        <color rgb="FF999999"/>
       </left>
       <right/>
       <top/>
@@ -579,7 +572,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color rgb="FFABABAB"/>
+        <color rgb="FF999999"/>
       </right>
       <top/>
       <bottom/>
@@ -587,14 +580,14 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFABABAB"/>
+        <color rgb="FF999999"/>
       </left>
       <right/>
       <top style="thin">
-        <color rgb="FFABABAB"/>
+        <color rgb="FF999999"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFABABAB"/>
+        <color rgb="FF999999"/>
       </bottom>
       <diagonal/>
     </border>
@@ -602,23 +595,23 @@
       <left/>
       <right/>
       <top style="thin">
-        <color rgb="FFABABAB"/>
+        <color rgb="FF999999"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFABABAB"/>
+        <color rgb="FF999999"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color rgb="FFABABAB"/>
+        <color rgb="FF999999"/>
       </right>
       <top style="thin">
-        <color rgb="FFABABAB"/>
+        <color rgb="FF999999"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFABABAB"/>
+        <color rgb="FF999999"/>
       </bottom>
       <diagonal/>
     </border>
@@ -626,18 +619,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="34">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -656,43 +648,137 @@
     <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" pivotButton="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" pivotButton="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCFE2F3"/>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="&quot;Aptos Narrow&quot;"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -706,7 +792,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Asus" refreshedDate="45954.597264467593" refreshedVersion="8" recordCount="16" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Usuario" refreshedDate="45955.529571874999" refreshedVersion="8" recordCount="16" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:F1000" sheet="4. Resultados acumulados"/>
   </cacheSource>
@@ -1005,6 +1091,18 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BBD0ABC9-47C1-487F-8655-53775B33F1AB}" name="Tabla1" displayName="Tabla1" ref="A1:D14" totalsRowShown="0" headerRowDxfId="0">
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{498D4C1F-D3A6-4049-A5C7-38728274724F}" name="Nombre de promoción" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{2B17F4D2-676C-443F-A921-7AA131C8DC1A}" name="Delegado" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{87127853-55E3-4D81-A02F-8D5DA41FBC53}" name="Grupo" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{086987CE-4C65-4811-8458-EF2B674C1F5A}" name="Número de jugadores" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -1210,7 +1308,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1221,18 +1319,18 @@
   <sheetPr codeName="Hoja2">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1250,25 +1348,19 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="4">
-        <v>11</v>
-      </c>
+      <c r="A2" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -1279,13 +1371,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D4" s="4">
         <v>11</v>
@@ -1293,10 +1385,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>11</v>
@@ -1307,13 +1399,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>6</v>
+        <v>13</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="D6" s="4">
         <v>11</v>
@@ -1321,13 +1413,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D7" s="4">
         <v>11</v>
@@ -1335,13 +1427,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>6</v>
+      <c r="C8" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="D8" s="4">
         <v>11</v>
@@ -1349,13 +1441,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D9" s="4">
         <v>11</v>
@@ -1363,13 +1455,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>6</v>
+      <c r="C10" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="D10" s="4">
         <v>11</v>
@@ -1377,13 +1469,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D11" s="4">
         <v>11</v>
@@ -1391,13 +1483,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>6</v>
+      <c r="C12" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="D12" s="4">
         <v>11</v>
@@ -1405,24 +1497,40 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D13" s="4">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="6"/>
+      <c r="A14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A15" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1000" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1433,34 +1541,36 @@
   </sheetPr>
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="4" max="4" width="26.109375" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
-        <v>28</v>
+        <v>127</v>
       </c>
       <c r="B2" s="4">
         <v>10000001</v>
@@ -2410,36 +2520,36 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="11">
+      <c r="A2" s="10">
         <v>45956</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="11">
         <v>0.41666666666666669</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -2459,10 +2569,10 @@
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="11">
+      <c r="A3" s="10">
         <v>45956</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="11">
         <v>0.44791666666666669</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -2482,10 +2592,10 @@
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="11">
+      <c r="A4" s="10">
         <v>45956</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="11">
         <v>0.47916666666666669</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -2505,10 +2615,10 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="11">
+      <c r="A5" s="10">
         <v>45956</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <v>0.53125</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -2528,10 +2638,10 @@
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="11">
+      <c r="A6" s="10">
         <v>45956</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="11">
         <v>0.5625</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -2543,18 +2653,18 @@
       <c r="E6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="13">
-        <v>1</v>
-      </c>
-      <c r="G6" s="13">
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="11">
+      <c r="A7" s="10">
         <v>45956</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="11">
         <v>0.59375</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -2566,10 +2676,10 @@
       <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="13">
-        <v>1</v>
-      </c>
-      <c r="G7" s="13">
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4">
         <v>1</v>
       </c>
       <c r="J7" s="2" t="s">
@@ -2583,8 +2693,8 @@
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="3" t="s">
         <v>99</v>
       </c>
@@ -2594,10 +2704,10 @@
       <c r="E8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="13">
-        <v>1</v>
-      </c>
-      <c r="G8" s="13">
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4">
         <v>1</v>
       </c>
       <c r="J8" s="2" t="s">
@@ -2611,8 +2721,8 @@
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="3" t="s">
         <v>100</v>
       </c>
@@ -2622,10 +2732,10 @@
       <c r="E9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="13">
-        <v>1</v>
-      </c>
-      <c r="G9" s="13">
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+      <c r="G9" s="4">
         <v>1</v>
       </c>
       <c r="J9" s="2" t="s">
@@ -2639,8 +2749,8 @@
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="3" t="s">
         <v>101</v>
       </c>
@@ -2650,10 +2760,10 @@
       <c r="E10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="13">
-        <v>1</v>
-      </c>
-      <c r="G10" s="13">
+      <c r="F10" s="4">
+        <v>1</v>
+      </c>
+      <c r="G10" s="4">
         <v>1</v>
       </c>
       <c r="J10" s="2" t="s">
@@ -2667,8 +2777,8 @@
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="3" t="s">
         <v>102</v>
       </c>
@@ -2678,10 +2788,10 @@
       <c r="E11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="13">
-        <v>1</v>
-      </c>
-      <c r="G11" s="13">
+      <c r="F11" s="4">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4">
         <v>1</v>
       </c>
       <c r="J11" s="2" t="s">
@@ -2695,8 +2805,8 @@
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="14"/>
-      <c r="B12" s="15"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="3" t="s">
         <v>103</v>
       </c>
@@ -2706,10 +2816,10 @@
       <c r="E12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="13">
-        <v>1</v>
-      </c>
-      <c r="G12" s="13">
+      <c r="F12" s="4">
+        <v>1</v>
+      </c>
+      <c r="G12" s="4">
         <v>1</v>
       </c>
       <c r="J12" s="2" t="s">
@@ -2723,8 +2833,8 @@
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="3" t="s">
         <v>104</v>
       </c>
@@ -2734,16 +2844,16 @@
       <c r="E13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="13">
-        <v>1</v>
-      </c>
-      <c r="G13" s="13">
+      <c r="F13" s="4">
+        <v>1</v>
+      </c>
+      <c r="G13" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="14"/>
-      <c r="B14" s="15"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -2751,8 +2861,8 @@
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="14"/>
-      <c r="B15" s="15"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -2769,8 +2879,8 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="14"/>
-      <c r="B16" s="15"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -2787,8 +2897,8 @@
       </c>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -2805,8 +2915,8 @@
       </c>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="14"/>
-      <c r="B18" s="15"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -2823,8 +2933,8 @@
       </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="14"/>
-      <c r="B19" s="15"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -2841,8 +2951,8 @@
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="14"/>
-      <c r="B20" s="15"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -2859,8 +2969,8 @@
       </c>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="14"/>
-      <c r="B21" s="15"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -2884,25 +2994,25 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="12" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3259,305 +3369,305 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.2">
-      <c r="A1" s="18"/>
-      <c r="B1" s="19" t="s">
+    <row r="1" spans="1:6" ht="12.75">
+      <c r="A1" s="14"/>
+      <c r="B1" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="21"/>
-    </row>
-    <row r="2" spans="1:6" ht="13.2">
-      <c r="A2" s="19" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="17"/>
+    </row>
+    <row r="2" spans="1:6" ht="12.75">
+      <c r="A2" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="19" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.2">
-      <c r="A3" s="18" t="s">
+    <row r="3" spans="1:6" ht="12.75">
+      <c r="A3" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="20">
         <v>4</v>
       </c>
-      <c r="C3" s="25">
+      <c r="C3" s="21">
         <v>3</v>
       </c>
-      <c r="D3" s="25">
-        <v>2</v>
-      </c>
-      <c r="E3" s="25">
-        <v>1</v>
-      </c>
-      <c r="F3" s="26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="13.2">
-      <c r="A4" s="27" t="s">
+      <c r="D3" s="21">
+        <v>2</v>
+      </c>
+      <c r="E3" s="21">
+        <v>1</v>
+      </c>
+      <c r="F3" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="12.75">
+      <c r="A4" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="24">
         <v>4</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="25">
         <v>5</v>
       </c>
-      <c r="D4" s="29">
-        <v>1</v>
-      </c>
-      <c r="E4" s="29">
+      <c r="D4" s="25">
+        <v>1</v>
+      </c>
+      <c r="E4" s="25">
         <v>4</v>
       </c>
-      <c r="F4" s="30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="13.2">
-      <c r="A5" s="27" t="s">
+      <c r="F4" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="12.75">
+      <c r="A5" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="24">
         <v>4</v>
       </c>
-      <c r="C5" s="29">
+      <c r="C5" s="25">
         <v>5</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="25">
         <v>4</v>
       </c>
-      <c r="E5" s="29">
-        <v>1</v>
-      </c>
-      <c r="F5" s="30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="13.2">
-      <c r="A6" s="27" t="s">
+      <c r="E5" s="25">
+        <v>1</v>
+      </c>
+      <c r="F5" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="12.75">
+      <c r="A6" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="24">
         <v>4</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="25">
         <v>3</v>
       </c>
-      <c r="D6" s="29">
-        <v>2</v>
-      </c>
-      <c r="E6" s="29">
-        <v>1</v>
-      </c>
-      <c r="F6" s="30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="13.2">
-      <c r="A7" s="27" t="s">
+      <c r="D6" s="25">
+        <v>2</v>
+      </c>
+      <c r="E6" s="25">
+        <v>1</v>
+      </c>
+      <c r="F6" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="12.75">
+      <c r="A7" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="28">
-        <v>2</v>
-      </c>
-      <c r="C7" s="29">
-        <v>2</v>
-      </c>
-      <c r="D7" s="29">
-        <v>2</v>
-      </c>
-      <c r="E7" s="29">
+      <c r="B7" s="24">
+        <v>2</v>
+      </c>
+      <c r="C7" s="25">
+        <v>2</v>
+      </c>
+      <c r="D7" s="25">
+        <v>2</v>
+      </c>
+      <c r="E7" s="25">
         <v>0</v>
       </c>
-      <c r="F7" s="30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="13.2">
-      <c r="A8" s="27" t="s">
+      <c r="F7" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="12.75">
+      <c r="A8" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="28">
-        <v>2</v>
-      </c>
-      <c r="C8" s="29">
+      <c r="B8" s="24">
+        <v>2</v>
+      </c>
+      <c r="C8" s="25">
         <v>3</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="25">
         <v>3</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="25">
         <v>0</v>
       </c>
-      <c r="F8" s="30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="13.2">
-      <c r="A9" s="27" t="s">
+      <c r="F8" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="12.75">
+      <c r="A9" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="28">
-        <v>2</v>
-      </c>
-      <c r="C9" s="29">
-        <v>2</v>
-      </c>
-      <c r="D9" s="29">
-        <v>2</v>
-      </c>
-      <c r="E9" s="29">
+      <c r="B9" s="24">
+        <v>2</v>
+      </c>
+      <c r="C9" s="25">
+        <v>2</v>
+      </c>
+      <c r="D9" s="25">
+        <v>2</v>
+      </c>
+      <c r="E9" s="25">
         <v>0</v>
       </c>
-      <c r="F9" s="30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="13.2">
-      <c r="A10" s="27" t="s">
+      <c r="F9" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="12.75">
+      <c r="A10" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="28">
-        <v>2</v>
-      </c>
-      <c r="C10" s="29">
+      <c r="B10" s="24">
+        <v>2</v>
+      </c>
+      <c r="C10" s="25">
         <v>3</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="25">
         <v>3</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="25">
         <v>0</v>
       </c>
-      <c r="F10" s="30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="13.2">
-      <c r="A11" s="27" t="s">
+      <c r="F10" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="12.75">
+      <c r="A11" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="28">
-        <v>1</v>
-      </c>
-      <c r="C11" s="29">
+      <c r="B11" s="24">
+        <v>1</v>
+      </c>
+      <c r="C11" s="25">
         <v>4</v>
       </c>
-      <c r="D11" s="29">
+      <c r="D11" s="25">
         <v>5</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11" s="25">
         <v>-1</v>
       </c>
-      <c r="F11" s="30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="13.2">
-      <c r="A12" s="27" t="s">
+      <c r="F11" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="12.75">
+      <c r="A12" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="28">
-        <v>1</v>
-      </c>
-      <c r="C12" s="29">
-        <v>2</v>
-      </c>
-      <c r="D12" s="29">
+      <c r="B12" s="24">
+        <v>1</v>
+      </c>
+      <c r="C12" s="25">
+        <v>2</v>
+      </c>
+      <c r="D12" s="25">
         <v>3</v>
       </c>
-      <c r="E12" s="29">
+      <c r="E12" s="25">
         <v>-1</v>
       </c>
-      <c r="F12" s="30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="13.2">
-      <c r="A13" s="27" t="s">
+      <c r="F12" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="12.75">
+      <c r="A13" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="28">
-        <v>1</v>
-      </c>
-      <c r="C13" s="29">
-        <v>1</v>
-      </c>
-      <c r="D13" s="29">
+      <c r="B13" s="24">
+        <v>1</v>
+      </c>
+      <c r="C13" s="25">
+        <v>1</v>
+      </c>
+      <c r="D13" s="25">
         <v>5</v>
       </c>
-      <c r="E13" s="29">
+      <c r="E13" s="25">
         <v>-4</v>
       </c>
-      <c r="F13" s="30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="13.2">
-      <c r="A14" s="27" t="s">
+      <c r="F13" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="12.75">
+      <c r="A14" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="28">
-        <v>1</v>
-      </c>
-      <c r="C14" s="29">
-        <v>2</v>
-      </c>
-      <c r="D14" s="29">
+      <c r="B14" s="24">
+        <v>1</v>
+      </c>
+      <c r="C14" s="25">
+        <v>2</v>
+      </c>
+      <c r="D14" s="25">
         <v>3</v>
       </c>
-      <c r="E14" s="29">
+      <c r="E14" s="25">
         <v>-1</v>
       </c>
-      <c r="F14" s="30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="13.2">
-      <c r="A15" s="27" t="s">
+      <c r="F14" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="12.75">
+      <c r="A15" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="30"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="26"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="B16" s="32">
+      <c r="B16" s="28">
         <v>28</v>
       </c>
-      <c r="C16" s="33">
+      <c r="C16" s="29">
         <v>35</v>
       </c>
-      <c r="D16" s="33">
+      <c r="D16" s="29">
         <v>35</v>
       </c>
-      <c r="E16" s="33">
+      <c r="E16" s="29">
         <v>0</v>
       </c>
-      <c r="F16" s="34">
+      <c r="F16" s="30">
         <v>24</v>
       </c>
     </row>
@@ -3575,22 +3685,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="13" t="s">
         <v>112</v>
       </c>
     </row>
@@ -3604,7 +3714,7 @@
       <c r="C2" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="10">
         <v>45955</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -3621,7 +3731,7 @@
       <c r="C3" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="10">
         <v>45957</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -3638,7 +3748,7 @@
       <c r="C4" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="10">
         <v>45958</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -3655,7 +3765,7 @@
       <c r="C5" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="10">
         <v>45960</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -3672,7 +3782,7 @@
       <c r="C6" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="10">
         <v>45962</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -3689,7 +3799,7 @@
       <c r="C7" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="10">
         <v>45963</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -3706,7 +3816,7 @@
       <c r="C8" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="10">
         <v>45964</v>
       </c>
       <c r="E8" s="3" t="s">

</xml_diff>